<commit_message>
Trip Detail Excel Basic
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="55">
   <si>
     <t>TestCase</t>
   </si>
@@ -164,17 +164,55 @@
   </si>
   <si>
     <t>Mật khẩu phải có ít nhất 8 ký tự</t>
+  </si>
+  <si>
+    <t>Number of Participants</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>EntryDate</t>
+  </si>
+  <si>
+    <t>ExitDate</t>
+  </si>
+  <si>
+    <t>Arrival Keyword</t>
+  </si>
+  <si>
+    <t>Arrival Option</t>
+  </si>
+  <si>
+    <t>ProcessingTime</t>
+  </si>
+  <si>
+    <t>Kiểm tra form chi tiết chuyến đi
+khi nhập đầy đủ thông tin hợp lệ</t>
+  </si>
+  <si>
+    <t>e_tourist|1MD</t>
+  </si>
+  <si>
+    <t>Indira</t>
+  </si>
+  <si>
+    <t>Indira Gandhi Int'l Airport</t>
+  </si>
+  <si>
+    <t>urgent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -797,13 +835,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1133,357 +1182,357 @@
   <sheetPr/>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.4444444444444"/>
-    <col min="2" max="2" customWidth="true" width="19.6666666666667"/>
-    <col min="3" max="3" customWidth="true" width="33.5555555555556"/>
-    <col min="4" max="4" customWidth="true" width="27.7777777777778"/>
-    <col min="5" max="5" customWidth="true" width="42.2222222222222"/>
-    <col min="6" max="6" customWidth="true" width="23.8888888888889"/>
-    <col min="7" max="7" customWidth="true" width="38.1111111111111"/>
-    <col min="8" max="8" customWidth="true" width="41.5555555555556"/>
-    <col min="9" max="9" customWidth="true" width="29.2222222222222"/>
-    <col min="10" max="11" customWidth="true" width="33.3333333333333"/>
-    <col min="12" max="15" customWidth="true" width="8.88888888888889"/>
+    <col min="1" max="1" width="14.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="19.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="33.5555555555556" customWidth="1"/>
+    <col min="4" max="4" width="27.7777777777778" customWidth="1"/>
+    <col min="5" max="5" width="42.2222222222222" customWidth="1"/>
+    <col min="6" max="6" width="23.8888888888889" customWidth="1"/>
+    <col min="7" max="7" width="38.1111111111111" customWidth="1"/>
+    <col min="8" max="8" width="41.5555555555556" customWidth="1"/>
+    <col min="9" max="9" width="29.2222222222222" customWidth="1"/>
+    <col min="10" max="11" width="33.3333333333333" customWidth="1"/>
+    <col min="12" max="15" width="8.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:11">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" ht="58" customHeight="1" spans="1:10">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" ht="63" customHeight="1" spans="1:10">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" ht="51" customHeight="1" spans="1:10">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>12345678</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="1" ht="55" customHeight="1" spans="1:10">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="5">
         <v>12345678</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="1" ht="55" customHeight="1" spans="1:10">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>123456</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" ht="52" customHeight="1" spans="1:10">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" ht="56" customHeight="1" spans="1:10">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" ht="54" customHeight="1" spans="1:10">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <v>12345678</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" ht="63" customHeight="1" spans="1:10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="5">
         <v>12345678</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" ht="46" customHeight="1" spans="1:10">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="5">
         <v>123456</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1497,181 +1546,277 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.4444444444444"/>
-    <col min="2" max="2" customWidth="true" width="19.6666666666667"/>
-    <col min="3" max="3" customWidth="true" width="33.5555555555556"/>
-    <col min="4" max="4" customWidth="true" width="27.7777777777778"/>
-    <col min="5" max="5" customWidth="true" width="42.2222222222222"/>
-    <col min="6" max="6" customWidth="true" width="23.8888888888889"/>
-    <col min="7" max="7" customWidth="true" width="38.1111111111111"/>
-    <col min="8" max="8" customWidth="true" width="41.5555555555556"/>
-    <col min="9" max="9" customWidth="true" width="29.2222222222222"/>
-    <col min="10" max="11" customWidth="true" width="33.3333333333333"/>
-    <col min="12" max="15" customWidth="true" width="8.88888888888889"/>
+    <col min="1" max="1" width="14.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="19.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="33.5555555555556" customWidth="1"/>
+    <col min="4" max="4" width="27.7777777777778" customWidth="1"/>
+    <col min="5" max="5" width="42.2222222222222" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.1111111111111" customWidth="1"/>
+    <col min="7" max="8" width="38.1111111111111" style="3" customWidth="1"/>
+    <col min="9" max="13" width="38.1111111111111" customWidth="1"/>
+    <col min="14" max="14" width="41.5555555555556" customWidth="1"/>
+    <col min="15" max="15" width="29.2222222222222" customWidth="1"/>
+    <col min="16" max="17" width="33.3333333333333" customWidth="1"/>
+    <col min="18" max="21" width="8.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:11">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:16">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" ht="58" customHeight="1" spans="1:10">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" ht="63" customHeight="1" spans="1:10">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" ht="51" customHeight="1" spans="1:10">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" customFormat="1" ht="55" customHeight="1" spans="1:10">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" customFormat="1" ht="55" customHeight="1" spans="1:10">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" ht="52" customHeight="1" spans="1:10">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
+    <row r="2" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6">
+        <v>45725</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="8">
+        <v>45910</v>
+      </c>
+      <c r="H2" s="8">
+        <v>45920</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" ht="63" customHeight="1" spans="1:16">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" ht="51" customHeight="1" spans="1:16">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+    </row>
+    <row r="5" customFormat="1" ht="55" customHeight="1" spans="1:16">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" customFormat="1" ht="55" customHeight="1" spans="1:16">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" ht="52" customHeight="1" spans="1:16">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" ht="56" customHeight="1" spans="1:10">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" ht="54" customHeight="1" spans="1:10">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" ht="63" customHeight="1" spans="1:10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" ht="46" customHeight="1" spans="1:10">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="9"/>
+    </row>
+    <row r="8" ht="56" customHeight="1" spans="1:16">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" ht="54" customHeight="1" spans="1:16">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" ht="63" customHeight="1" spans="1:16">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+    </row>
+    <row r="11" ht="46" customHeight="1" spans="1:16">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Passenger Info Page With 2 People
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="10440" activeTab="2"/>
+    <workbookView windowWidth="22188" windowHeight="10440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="98">
   <si>
     <t>TestCase</t>
   </si>
@@ -189,7 +189,8 @@
   </si>
   <si>
     <t>Kiểm tra form chi tiết chuyến đi
-khi nhập đầy đủ thông tin hợp lệ</t>
+khi nhập đầy đủ thông tin hợp lệ 
+với trường hợp 1 hành khách</t>
   </si>
   <si>
     <t>e_tourist|1MD</t>
@@ -205,6 +206,11 @@
   </si>
   <si>
     <t>Form thông tin hành khách hiển thị</t>
+  </si>
+  <si>
+    <t>Kiểm tra form chi tiết chuyến đi
+khi nhập đầy đủ thông tin hợp lệ 
+với trường hợp nhiều hành khách</t>
   </si>
   <si>
     <t>Kiểm tra form chi tiết chuyến đi
@@ -277,6 +283,9 @@
     <t>Không tìm thấy sân bay</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>Kiểm tra form chi tiết chuyến đi
 khi nhập sai thời gian xử lí ứng với ngày
 xuất cảnh</t>
@@ -286,6 +295,63 @@
   </si>
   <si>
     <t>Thời gian xử lí không phù hợp</t>
+  </si>
+  <si>
+    <t>Fullname</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Dob</t>
+  </si>
+  <si>
+    <t>Nation Key</t>
+  </si>
+  <si>
+    <t>Nation Option</t>
+  </si>
+  <si>
+    <t>Nationality Key</t>
+  </si>
+  <si>
+    <t>Nationality Option</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>Expired</t>
+  </si>
+  <si>
+    <t>Passport Image</t>
+  </si>
+  <si>
+    <t>Portrait Image</t>
+  </si>
+  <si>
+    <t>Kiểm tra form thông tin 
+hành khách khi nhập đầy đủ 
+thông tin hợp lệ với trường hợp
+2 hành khách</t>
+  </si>
+  <si>
+    <t>Khach Hang</t>
+  </si>
+  <si>
+    <t>Vi</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>111111111111</t>
+  </si>
+  <si>
+    <t>C:\Users\ADMIN\Downloads\image.jpg</t>
+  </si>
+  <si>
+    <t>Form thông tin liên lạc hiển thị</t>
   </si>
 </sst>
 </file>
@@ -466,7 +532,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +542,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,7 +868,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -820,16 +892,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -838,105 +910,115 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -946,7 +1028,25 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1289,338 +1389,338 @@
     <col min="12" max="15" width="8.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="8" customFormat="1" spans="1:11">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" ht="58" customHeight="1" spans="1:10">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" ht="63" customHeight="1" spans="1:10">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" ht="51" customHeight="1" spans="1:10">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>12345678</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="1" ht="55" customHeight="1" spans="1:10">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>12345678</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="1" ht="55" customHeight="1" spans="1:10">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>123456</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" ht="52" customHeight="1" spans="1:10">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" ht="56" customHeight="1" spans="1:10">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" ht="54" customHeight="1" spans="1:10">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>12345678</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" ht="63" customHeight="1" spans="1:10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>12345678</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" ht="46" customHeight="1" spans="1:10">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>123456</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1634,10 +1734,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1646,546 +1746,636 @@
     <col min="2" max="2" width="19.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="33.5555555555556" customWidth="1"/>
     <col min="4" max="4" width="27.7777777777778" customWidth="1"/>
-    <col min="5" max="5" width="42.2222222222222" style="3" customWidth="1"/>
+    <col min="5" max="5" width="42.2222222222222" style="10" customWidth="1"/>
     <col min="6" max="6" width="28.1111111111111" customWidth="1"/>
-    <col min="7" max="8" width="38.1111111111111" style="4" customWidth="1"/>
+    <col min="7" max="8" width="38.1111111111111" style="2" customWidth="1"/>
     <col min="9" max="12" width="38.1111111111111" customWidth="1"/>
-    <col min="13" max="13" width="38.1111111111111" style="5" customWidth="1"/>
-    <col min="14" max="14" width="41.5555555555556" style="6" customWidth="1"/>
+    <col min="13" max="13" width="38.1111111111111" style="1" customWidth="1"/>
+    <col min="14" max="14" width="41.5555555555556" style="11" customWidth="1"/>
     <col min="15" max="15" width="29.2222222222222" customWidth="1"/>
     <col min="16" max="17" width="33.3333333333333" customWidth="1"/>
     <col min="18" max="21" width="8.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:16">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="8" customFormat="1" spans="1:16">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8">
+      <c r="A2" s="6"/>
+      <c r="B2" s="12">
         <v>45725</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9">
+      <c r="D2" s="6"/>
+      <c r="E2" s="13">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="14">
         <v>45910</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="14">
         <v>45920</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
+      <c r="M2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
     </row>
     <row r="3" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8">
+      <c r="A3" s="6"/>
+      <c r="B3" s="12">
+        <v>45725</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="13">
+        <v>3</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="14">
+        <v>45910</v>
+      </c>
+      <c r="H3" s="14">
+        <v>45920</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A4" s="6"/>
+      <c r="B4" s="12">
         <v>45756</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9" t="s">
+      <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G4" s="14">
         <v>45910</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H4" s="14">
         <v>45920</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8">
+      <c r="L4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A5" s="6"/>
+      <c r="B5" s="12">
         <v>45756</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="13">
+        <v>11</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="14">
+        <v>45910</v>
+      </c>
+      <c r="H5" s="14">
+        <v>45920</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="9">
-        <v>11</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="M5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A6" s="6"/>
+      <c r="B6" s="12">
+        <v>45756</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="13">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14">
+        <v>45910</v>
+      </c>
+      <c r="H6" s="14">
+        <v>45920</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A7" s="6"/>
+      <c r="B7" s="12">
+        <v>45756</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="14">
+        <v>45910</v>
+      </c>
+      <c r="H7" s="14">
+        <v>45920</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A8" s="6"/>
+      <c r="B8" s="12">
+        <v>45756</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
+        <v>45920</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A9" s="6"/>
+      <c r="B9" s="12">
+        <v>45756</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="14">
+        <v>45903</v>
+      </c>
+      <c r="H9" s="14">
+        <v>45920</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A10" s="6"/>
+      <c r="B10" s="12">
+        <v>45756</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="14">
         <v>45910</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H10" s="14"/>
+      <c r="I10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A11" s="6"/>
+      <c r="B11" s="12">
+        <v>45756</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="13">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="14">
+        <v>45910</v>
+      </c>
+      <c r="H11" s="14">
+        <v>45908</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A12" s="6"/>
+      <c r="B12" s="12">
+        <v>45756</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="14">
+        <v>45910</v>
+      </c>
+      <c r="H12" s="14">
         <v>45920</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" s="9" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16">
+        <v>45756</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="18">
+        <v>45910</v>
+      </c>
+      <c r="H13" s="18">
+        <v>45920</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A14" s="6"/>
+      <c r="B14" s="12">
+        <v>45756</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="14">
+        <v>45904</v>
+      </c>
+      <c r="H14" s="14">
+        <v>45920</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="9">
-        <v>1</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10">
-        <v>45910</v>
-      </c>
-      <c r="H5" s="10">
-        <v>45920</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="10">
-        <v>45910</v>
-      </c>
-      <c r="H6" s="10">
-        <v>45920</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="9">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10">
-        <v>45920</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="10">
-        <v>45903</v>
-      </c>
-      <c r="H8" s="10">
-        <v>45920</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="10">
-        <v>45910</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="10">
-        <v>45910</v>
-      </c>
-      <c r="H10" s="10">
-        <v>45908</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="9">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="10">
-        <v>45910</v>
-      </c>
-      <c r="H11" s="10">
-        <v>45920</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M11" s="7"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-    </row>
-    <row r="12" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="10">
-        <v>45910</v>
-      </c>
-      <c r="H12" s="10">
-        <v>45920</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="M12" s="7"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-    </row>
-    <row r="13" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8">
-        <v>45756</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="9">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="10">
-        <v>45904</v>
-      </c>
-      <c r="H13" s="10">
-        <v>45920</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="7" t="s">
+      <c r="K14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="M13" s="7"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" ht="63" customHeight="1" spans="1:16">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" ht="46" customHeight="1" spans="1:16">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" ht="63" customHeight="1" spans="1:16">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" ht="46" customHeight="1" spans="1:16">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2197,80 +2387,139 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="18.8888888888889" customWidth="1"/>
     <col min="2" max="2" width="26.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="29.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="32.7777777777778" customWidth="1"/>
-    <col min="5" max="5" width="21.3333333333333" customWidth="1"/>
-    <col min="6" max="6" width="14.7777777777778" customWidth="1"/>
-    <col min="7" max="7" width="20.5555555555556" customWidth="1"/>
+    <col min="5" max="5" width="23.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="19.5555555555556" customWidth="1"/>
+    <col min="7" max="7" width="20.5555555555556" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.3333333333333" customWidth="1"/>
     <col min="9" max="9" width="20.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="24.5555555555556" customWidth="1"/>
-    <col min="11" max="11" width="21.5555555555556" customWidth="1"/>
-    <col min="12" max="12" width="21.3333333333333" customWidth="1"/>
-    <col min="13" max="13" width="28.2222222222222" customWidth="1"/>
-    <col min="14" max="14" width="12.2222222222222" customWidth="1"/>
-    <col min="15" max="15" width="11.8888888888889" customWidth="1"/>
-    <col min="16" max="16" width="20.2222222222222" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="11" max="12" width="24.5555555555556" customWidth="1"/>
+    <col min="13" max="13" width="21.5555555555556" style="2" customWidth="1"/>
+    <col min="14" max="14" width="42" customWidth="1"/>
+    <col min="15" max="15" width="45.7777777777778" customWidth="1"/>
+    <col min="16" max="16" width="33.5555555555556" customWidth="1"/>
+    <col min="17" max="17" width="44.5555555555556" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5555555555556" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.8888888888889" customWidth="1"/>
+    <col min="20" max="20" width="23.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1" spans="1:16">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="22" customHeight="1" spans="1:20">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="76" customHeight="1" spans="2:16">
+      <c r="B2" s="5">
+        <v>45756</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="7">
+        <v>37837</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" s="7">
+        <v>46022</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional TripDetail No Fill All Mandatory Field
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="99">
   <si>
     <t>TestCase</t>
   </si>
@@ -209,11 +209,6 @@
   </si>
   <si>
     <t>Kiểm tra form chi tiết chuyến đi
-khi nhập đầy đủ thông tin hợp lệ 
-với trường hợp nhiều hành khách</t>
-  </si>
-  <si>
-    <t>Kiểm tra form chi tiết chuyến đi
 khi nhập thiếu trường số lượng khách</t>
   </si>
   <si>
@@ -295,6 +290,13 @@
   </si>
   <si>
     <t>Thời gian xử lí không phù hợp</t>
+  </si>
+  <si>
+    <t>Kiểm tra form chi tiết chuyến đi
+khi không nhập trường nào</t>
+  </si>
+  <si>
+    <t>Số lượng khách là bắt buộc;Mục đích chuyến đi là bắt buộc;Ngày nhập cảnh là bắt buộc;Ngày xuất cảnh là bắt buộc;Cảng nhập cảnh là bắt buộc</t>
   </si>
   <si>
     <t>Fullname</t>
@@ -532,7 +534,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,6 +550,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,7 +876,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -892,16 +900,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -910,89 +918,89 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1014,7 +1022,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1028,19 +1036,37 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1370,7 +1396,7 @@
   <sheetPr/>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1:I1"/>
     </sheetView>
   </sheetViews>
@@ -1597,7 +1623,7 @@
       <c r="H7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="26" t="s">
         <v>17</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -1734,10 +1760,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1852,15 +1878,13 @@
     <row r="3" customFormat="1" ht="58" customHeight="1" spans="1:16">
       <c r="A3" s="6"/>
       <c r="B3" s="12">
-        <v>45725</v>
+        <v>45756</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>56</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="13">
-        <v>3</v>
-      </c>
+      <c r="E3" s="13"/>
       <c r="F3" s="13" t="s">
         <v>51</v>
       </c>
@@ -1880,10 +1904,10 @@
         <v>54</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>17</v>
@@ -1897,10 +1921,12 @@
         <v>45756</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="13"/>
+      <c r="E4" s="13">
+        <v>11</v>
+      </c>
       <c r="F4" s="13" t="s">
         <v>51</v>
       </c>
@@ -1920,10 +1946,10 @@
         <v>54</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>17</v>
@@ -1941,11 +1967,9 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="13">
-        <v>11</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>51</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F5" s="13"/>
       <c r="G5" s="14">
         <v>45910</v>
       </c>
@@ -1962,10 +1986,10 @@
         <v>54</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>17</v>
@@ -1979,13 +2003,15 @@
         <v>45756</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="13">
         <v>1</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="G6" s="14">
         <v>45910</v>
       </c>
@@ -2002,10 +2028,10 @@
         <v>54</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>17</v>
@@ -2019,18 +2045,16 @@
         <v>45756</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="13">
         <v>1</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="14">
-        <v>45910</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G7" s="14"/>
       <c r="H7" s="14">
         <v>45920</v>
       </c>
@@ -2044,10 +2068,10 @@
         <v>54</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>17</v>
@@ -2061,7 +2085,7 @@
         <v>45756</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="13">
@@ -2070,7 +2094,9 @@
       <c r="F8" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="14">
+        <v>45903</v>
+      </c>
       <c r="H8" s="14">
         <v>45920</v>
       </c>
@@ -2084,10 +2110,10 @@
         <v>54</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>17</v>
@@ -2101,7 +2127,7 @@
         <v>45756</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="13">
@@ -2111,11 +2137,9 @@
         <v>51</v>
       </c>
       <c r="G9" s="14">
-        <v>45903</v>
-      </c>
-      <c r="H9" s="14">
-        <v>45920</v>
-      </c>
+        <v>45910</v>
+      </c>
+      <c r="H9" s="14"/>
       <c r="I9" s="6" t="s">
         <v>52</v>
       </c>
@@ -2126,10 +2150,10 @@
         <v>54</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>17</v>
@@ -2143,7 +2167,7 @@
         <v>45756</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="13">
@@ -2155,7 +2179,9 @@
       <c r="G10" s="14">
         <v>45910</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14">
+        <v>45908</v>
+      </c>
       <c r="I10" s="6" t="s">
         <v>52</v>
       </c>
@@ -2166,10 +2192,10 @@
         <v>54</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>17</v>
@@ -2196,22 +2222,18 @@
         <v>45910</v>
       </c>
       <c r="H11" s="14">
-        <v>45908</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>53</v>
-      </c>
+        <v>45920</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="6" t="s">
         <v>54</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>17</v>
@@ -2219,129 +2241,119 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A12" s="6"/>
-      <c r="B12" s="12">
+    <row r="12" s="9" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16">
         <v>45756</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="18">
+        <v>45910</v>
+      </c>
+      <c r="H12" s="18">
+        <v>45920</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="M12" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13">
+      <c r="N12" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+    </row>
+    <row r="13" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="A13" s="19"/>
+      <c r="B13" s="20">
+        <v>45756</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="21">
         <v>1</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F13" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="14">
-        <v>45910</v>
-      </c>
-      <c r="H12" s="14">
+      <c r="G13" s="22">
+        <v>45905</v>
+      </c>
+      <c r="H13" s="22">
         <v>45920</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" s="9" customFormat="1" ht="58" customHeight="1" spans="1:16">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16">
-        <v>45756</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="17">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="18">
-        <v>45910</v>
-      </c>
-      <c r="H13" s="18">
-        <v>45920</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L13" s="15" t="s">
+      <c r="I13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="M13" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-    </row>
-    <row r="14" customFormat="1" ht="58" customHeight="1" spans="1:16">
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" customFormat="1" ht="74" customHeight="1" spans="1:16">
       <c r="A14" s="6"/>
       <c r="B14" s="12">
-        <v>45756</v>
+        <v>45786</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="13">
-        <v>1</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="14">
-        <v>45904</v>
-      </c>
-      <c r="H14" s="14">
-        <v>45920</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" ht="63" customHeight="1" spans="1:16">
+    <row r="15" ht="46" customHeight="1" spans="1:16">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2359,24 +2371,6 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" ht="46" customHeight="1" spans="1:16">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2390,7 +2384,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -2430,37 +2424,37 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>6</v>
@@ -2483,10 +2477,10 @@
         <v>45756</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
@@ -2495,31 +2489,31 @@
         <v>37837</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L2" s="21" t="s">
         <v>95</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>96</v>
       </c>
       <c r="M2" s="7">
         <v>46022</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>